<commit_message>
Little fix on students
</commit_message>
<xml_diff>
--- a/resource/uploads/import/skeleton/学生贡献度.xlsx
+++ b/resource/uploads/import/skeleton/学生贡献度.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangyang/PycharmProjects/Uranus/resource/uploads/import/skeleton/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -451,7 +451,7 @@
         <v>15211003</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>